<commit_message>
version of default just before Odata is added
</commit_message>
<xml_diff>
--- a/src/test/resources/bulk/image_manifest2.xlsx
+++ b/src/test/resources/bulk/image_manifest2.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="21075" windowHeight="10035"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="21080" windowHeight="10040"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,27 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>tDAR</author>
+  </authors>
+  <commentList>
+    <comment ref="R1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">An Institutional creator/ author/ sponsor's / etc. </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
@@ -104,9 +125,6 @@
     <t>publisherLocation</t>
   </si>
   <si>
-    <t>publisher</t>
-  </si>
-  <si>
     <t>isbn</t>
   </si>
   <si>
@@ -138,6 +156,9 @@
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>Publisher Institution Name</t>
   </si>
 </sst>
 </file>
@@ -210,7 +231,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -218,6 +239,9 @@
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,16 +544,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" ht="37">
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
@@ -540,7 +564,7 @@
         <v>18</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>19</v>
@@ -581,38 +605,38 @@
       <c r="Q1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="S1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="AB1" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="AC1" s="4" t="s">
         <v>2</v>
@@ -621,7 +645,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" ht="56">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -667,7 +691,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" ht="84">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -720,6 +744,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -734,7 +759,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -751,7 +776,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>